<commit_message>
Cleaned up cards and added Done button
</commit_message>
<xml_diff>
--- a/cheat-card/cheat-card.xlsx
+++ b/cheat-card/cheat-card.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s0041664\Documents\Development\HTML5\blackjack.js\cheat-card\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Development\HTML5\blackjack.js\cheat-card\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hard" sheetId="4" r:id="rId1"/>
     <sheet name="Pair" sheetId="2" r:id="rId2"/>
     <sheet name="Soft" sheetId="1" r:id="rId3"/>
+    <sheet name="Soft (old)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="49">
   <si>
     <t>Ace</t>
   </si>
@@ -159,12 +160,33 @@
   </si>
   <si>
     <t>D &gt;= +4/Hit</t>
+  </si>
+  <si>
+    <t>A-8</t>
+  </si>
+  <si>
+    <t>A-7</t>
+  </si>
+  <si>
+    <t>A-6</t>
+  </si>
+  <si>
+    <t>A-5</t>
+  </si>
+  <si>
+    <t>A-4</t>
+  </si>
+  <si>
+    <t>A-3</t>
+  </si>
+  <si>
+    <t>A-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -259,7 +281,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="249">
+  <dxfs count="89">
     <dxf>
       <fill>
         <patternFill>
@@ -354,12 +376,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF9B367"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBEF92B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF29EF8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFF6969"/>
         </patternFill>
       </fill>
     </dxf>
@@ -395,33 +438,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF6969"/>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -519,12 +541,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF9B367"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBEF92B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF29EF8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFF6969"/>
         </patternFill>
       </fill>
     </dxf>
@@ -601,33 +644,33 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF6969"/>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF9B367"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBEF92B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF29EF8A"/>
         </patternFill>
       </fill>
     </dxf>
@@ -637,7 +680,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFF6969"/>
         </patternFill>
       </fill>
     </dxf>
@@ -673,33 +716,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF6969"/>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -797,12 +819,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF9B367"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBEF92B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF29EF8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFF6969"/>
         </patternFill>
       </fill>
     </dxf>
@@ -896,1312 +939,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9B367"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBEF92B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF29EF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2535,7 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
@@ -2971,165 +1708,165 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:L12">
-    <cfRule type="cellIs" dxfId="89" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="52" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="53" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="54" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="55" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="56" operator="equal">
       <formula>"+4"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:G5">
-    <cfRule type="cellIs" dxfId="84" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="48" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="49" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="50" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="51" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:L6">
-    <cfRule type="cellIs" dxfId="80" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="44" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="45" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="46" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="47" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:G7 E8:G8">
-    <cfRule type="cellIs" dxfId="76" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="40" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="41" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="42" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="43" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:G8">
-    <cfRule type="cellIs" dxfId="72" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="36" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="37" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="38" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="39" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:K9">
-    <cfRule type="cellIs" dxfId="63" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="27" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="28" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="29" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="30" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:J10">
-    <cfRule type="cellIs" dxfId="55" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="19" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="20" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="21" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="22" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:G11">
-    <cfRule type="cellIs" dxfId="51" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="15" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="16" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="17" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="18" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="47" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="11" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="12" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="13" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="14" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="42" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="8" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="9" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:N10">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="3" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="4" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
       <formula>"+4"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3566,92 +2303,92 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:L12">
-    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="23" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="24" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="25" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="26" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="27" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:G5">
-    <cfRule type="cellIs" dxfId="28" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="19" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="20" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="21" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="22" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:L6">
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="14" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="15" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:G7">
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:G8">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:N8">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3661,6 +2398,361 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="4.42578125" style="2" customWidth="1"/>
+    <col min="3" max="12" width="4.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="4.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:N2 C3:M8 C9:N12 C17:N1048576 C13:M16 N5:N8">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"H"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
+      <formula>"D/H"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
+      <formula>"D/S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5:O8">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"H"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>"D/H"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>"D/S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O16"/>
   <sheetViews>
@@ -3994,13 +3086,13 @@
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"D/H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"D/S"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>